<commit_message>
se modificó archivo1 y hoja1. Sea agregó presentacion1
</commit_message>
<xml_diff>
--- a/hoja1.xlsx
+++ b/hoja1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>X</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>r</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -357,68 +360,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7">
         <v>6.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se modeificó después de clonar archivo1 y hoja1
</commit_message>
<xml_diff>
--- a/hoja1.xlsx
+++ b/hoja1.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDDA096-AD18-4539-8CBA-BD81B2E82835}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="3720" yWindow="750" windowWidth="13335" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>X</t>
   </si>
@@ -43,12 +44,18 @@
   </si>
   <si>
     <t>Z</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,11 +366,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,6 +452,28 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>6.9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>10.5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
editando archivo en excel
</commit_message>
<xml_diff>
--- a/hoja1.xlsx
+++ b/hoja1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDDA096-AD18-4539-8CBA-BD81B2E82835}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAB41ED-9CBC-4FE8-B378-14CA38AC15DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="750" windowWidth="13335" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1620" windowWidth="10200" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>X</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
 </sst>
 </file>
@@ -367,15 +370,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -385,8 +388,11 @@
       <c r="C1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -396,8 +402,11 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -407,8 +416,11 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -418,8 +430,11 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -429,19 +444,25 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>7.5</v>
+        <v>11.5</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -451,8 +472,11 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -462,8 +486,11 @@
       <c r="C8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -472,6 +499,9 @@
       </c>
       <c r="C9" t="s">
         <v>3</v>
+      </c>
+      <c r="D9">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregando última línea en excel
</commit_message>
<xml_diff>
--- a/hoja1.xlsx
+++ b/hoja1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAB41ED-9CBC-4FE8-B378-14CA38AC15DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C78FED-7686-4CE4-8FC1-6744B50AE886}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="690" yWindow="1620" windowWidth="10200" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t>X</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>xcv</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,6 +507,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
editando última línea excel desde la rama1
</commit_message>
<xml_diff>
--- a/hoja1.xlsx
+++ b/hoja1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAB41ED-9CBC-4FE8-B378-14CA38AC15DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1170D379-6822-4CD2-92BE-CBF2C05B6052}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="690" yWindow="1620" windowWidth="10200" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>X</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>W</t>
+  </si>
+  <si>
+    <t>aaaa</t>
   </si>
 </sst>
 </file>
@@ -370,10 +373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,6 +507,17 @@
         <v>17</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
editando por defecto excel en rama1
</commit_message>
<xml_diff>
--- a/hoja1.xlsx
+++ b/hoja1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1170D379-6822-4CD2-92BE-CBF2C05B6052}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EB69E7-65AF-4788-8955-26247A99F2B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="1620" windowWidth="10200" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7920" yWindow="1710" windowWidth="10200" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -376,7 +376,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>